<commit_message>
waitm-645: add missing close after cancel lab request modal
</commit_message>
<xml_diff>
--- a/packages/sync-server/__tests__/importers/refdata-valid.xlsx
+++ b/packages/sync-server/__tests__/importers/refdata-valid.xlsx
@@ -952,7 +952,7 @@
     <t>labSampleSite-Right-upper-arm</t>
   </si>
   <si>
-    <t xml:space="preserve">Rightupperarm </t>
+    <t>Rightupperarm</t>
   </si>
   <si>
     <t xml:space="preserve">Right upper arm </t>
@@ -1769,7 +1769,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1819,12 +1819,6 @@
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -3503,10 +3497,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="14.5" style="22" customWidth="1"/>
-    <col min="3" max="3" width="77.6719" style="22" customWidth="1"/>
-    <col min="4" max="5" width="14.5" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="22" customWidth="1"/>
+    <col min="1" max="2" width="14.5" style="20" customWidth="1"/>
+    <col min="3" max="3" width="77.6719" style="20" customWidth="1"/>
+    <col min="4" max="5" width="14.5" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -3669,10 +3663,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="14.5" style="23" customWidth="1"/>
-    <col min="3" max="3" width="28.8516" style="23" customWidth="1"/>
-    <col min="4" max="5" width="14.5" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="23" customWidth="1"/>
+    <col min="1" max="2" width="14.5" style="21" customWidth="1"/>
+    <col min="3" max="3" width="28.8516" style="21" customWidth="1"/>
+    <col min="4" max="5" width="14.5" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -3835,10 +3829,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="14.5" style="24" customWidth="1"/>
-    <col min="3" max="3" width="168.352" style="24" customWidth="1"/>
-    <col min="4" max="5" width="14.5" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="24" customWidth="1"/>
+    <col min="1" max="2" width="14.5" style="22" customWidth="1"/>
+    <col min="3" max="3" width="168.352" style="22" customWidth="1"/>
+    <col min="4" max="5" width="14.5" style="22" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -4001,9 +3995,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="29.5" style="25" customWidth="1"/>
-    <col min="2" max="5" width="14.5" style="25" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="25" customWidth="1"/>
+    <col min="1" max="1" width="29.5" style="23" customWidth="1"/>
+    <col min="2" max="5" width="14.5" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -4123,11 +4117,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="36.5" style="26" customWidth="1"/>
-    <col min="2" max="2" width="14.5" style="26" customWidth="1"/>
-    <col min="3" max="3" width="29.1719" style="26" customWidth="1"/>
-    <col min="4" max="5" width="14.5" style="26" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="26" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="24" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="24" customWidth="1"/>
+    <col min="3" max="3" width="29.1719" style="24" customWidth="1"/>
+    <col min="4" max="5" width="14.5" style="24" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -4498,15 +4492,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17.1719" style="27" customWidth="1"/>
-    <col min="2" max="2" width="20.3516" style="27" customWidth="1"/>
-    <col min="3" max="3" width="15.8516" style="27" customWidth="1"/>
-    <col min="4" max="4" width="21.6719" style="27" customWidth="1"/>
-    <col min="5" max="6" width="14.5" style="27" customWidth="1"/>
-    <col min="7" max="7" width="14" style="27" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="27" customWidth="1"/>
-    <col min="9" max="9" width="46.5" style="27" customWidth="1"/>
-    <col min="10" max="16384" width="14.5" style="27" customWidth="1"/>
+    <col min="1" max="1" width="17.1719" style="25" customWidth="1"/>
+    <col min="2" max="2" width="20.3516" style="25" customWidth="1"/>
+    <col min="3" max="3" width="15.8516" style="25" customWidth="1"/>
+    <col min="4" max="4" width="21.6719" style="25" customWidth="1"/>
+    <col min="5" max="6" width="14.5" style="25" customWidth="1"/>
+    <col min="7" max="7" width="14" style="25" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="25" customWidth="1"/>
+    <col min="9" max="9" width="46.5" style="25" customWidth="1"/>
+    <col min="10" max="16384" width="14.5" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -15702,17 +15696,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6667" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="34.6719" style="28" customWidth="1"/>
-    <col min="2" max="2" width="34.3516" style="28" customWidth="1"/>
-    <col min="3" max="4" width="10.6719" style="28" customWidth="1"/>
-    <col min="5" max="5" width="25.6719" style="28" customWidth="1"/>
-    <col min="6" max="7" width="10.6719" style="28" customWidth="1"/>
-    <col min="8" max="8" width="12.6719" style="28" customWidth="1"/>
-    <col min="9" max="9" width="17.8516" style="28" customWidth="1"/>
-    <col min="10" max="10" width="34" style="28" customWidth="1"/>
-    <col min="11" max="11" width="26.5" style="28" customWidth="1"/>
-    <col min="12" max="12" width="33.8516" style="28" customWidth="1"/>
-    <col min="13" max="16384" width="10.6719" style="28" customWidth="1"/>
+    <col min="1" max="1" width="34.6719" style="26" customWidth="1"/>
+    <col min="2" max="2" width="34.3516" style="26" customWidth="1"/>
+    <col min="3" max="4" width="10.6719" style="26" customWidth="1"/>
+    <col min="5" max="5" width="25.6719" style="26" customWidth="1"/>
+    <col min="6" max="7" width="10.6719" style="26" customWidth="1"/>
+    <col min="8" max="8" width="12.6719" style="26" customWidth="1"/>
+    <col min="9" max="9" width="17.8516" style="26" customWidth="1"/>
+    <col min="10" max="10" width="34" style="26" customWidth="1"/>
+    <col min="11" max="11" width="26.5" style="26" customWidth="1"/>
+    <col min="12" max="12" width="33.8516" style="26" customWidth="1"/>
+    <col min="13" max="16384" width="10.6719" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -15760,7 +15754,7 @@
       <c r="B2" t="s" s="2">
         <v>509</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="27">
         <v>37665</v>
       </c>
       <c r="D2" t="s" s="2">
@@ -15798,7 +15792,7 @@
       <c r="B3" t="s" s="2">
         <v>516</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="27">
         <v>37665</v>
       </c>
       <c r="D3" t="s" s="2">
@@ -15942,15 +15936,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6667" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="27.3516" style="30" customWidth="1"/>
-    <col min="2" max="2" width="12.8516" style="30" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="30" customWidth="1"/>
-    <col min="4" max="4" width="10.6719" style="30" customWidth="1"/>
-    <col min="5" max="5" width="17.6719" style="30" customWidth="1"/>
-    <col min="6" max="6" width="25.6719" style="30" customWidth="1"/>
-    <col min="7" max="7" width="10.6719" style="30" customWidth="1"/>
-    <col min="8" max="8" width="18.1719" style="30" customWidth="1"/>
-    <col min="9" max="16384" width="10.6719" style="30" customWidth="1"/>
+    <col min="1" max="1" width="27.3516" style="28" customWidth="1"/>
+    <col min="2" max="2" width="12.8516" style="28" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="28" customWidth="1"/>
+    <col min="4" max="4" width="10.6719" style="28" customWidth="1"/>
+    <col min="5" max="5" width="17.6719" style="28" customWidth="1"/>
+    <col min="6" max="6" width="25.6719" style="28" customWidth="1"/>
+    <col min="7" max="7" width="10.6719" style="28" customWidth="1"/>
+    <col min="8" max="8" width="18.1719" style="28" customWidth="1"/>
+    <col min="9" max="16384" width="10.6719" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -17246,251 +17240,251 @@
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" t="s" s="17">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="17">
+      <c r="B1" t="s" s="2">
         <v>114</v>
       </c>
-      <c r="C1" t="s" s="17">
+      <c r="C1" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="17">
+      <c r="A2" t="s" s="2">
         <v>239</v>
       </c>
-      <c r="B2" t="s" s="17">
+      <c r="B2" t="s" s="2">
         <v>240</v>
       </c>
-      <c r="C2" t="s" s="17">
+      <c r="C2" t="s" s="2">
         <v>240</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="17">
+      <c r="A3" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="B3" t="s" s="17">
+      <c r="B3" t="s" s="2">
         <v>242</v>
       </c>
-      <c r="C3" t="s" s="17">
+      <c r="C3" t="s" s="2">
         <v>243</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="17">
+      <c r="A4" t="s" s="2">
         <v>244</v>
       </c>
-      <c r="B4" t="s" s="17">
+      <c r="B4" t="s" s="2">
         <v>245</v>
       </c>
-      <c r="C4" t="s" s="17">
+      <c r="C4" t="s" s="2">
         <v>246</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="17">
+      <c r="A5" t="s" s="2">
         <v>247</v>
       </c>
-      <c r="B5" t="s" s="17">
+      <c r="B5" t="s" s="2">
         <v>248</v>
       </c>
-      <c r="C5" t="s" s="17">
+      <c r="C5" t="s" s="2">
         <v>249</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="17">
+      <c r="A6" t="s" s="2">
         <v>250</v>
       </c>
-      <c r="B6" t="s" s="17">
+      <c r="B6" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="C6" t="s" s="17">
+      <c r="C6" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="17">
+      <c r="A7" t="s" s="2">
         <v>253</v>
       </c>
-      <c r="B7" t="s" s="17">
+      <c r="B7" t="s" s="2">
         <v>254</v>
       </c>
-      <c r="C7" t="s" s="17">
+      <c r="C7" t="s" s="2">
         <v>255</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" t="s" s="17">
+      <c r="A8" t="s" s="2">
         <v>256</v>
       </c>
-      <c r="B8" t="s" s="17">
+      <c r="B8" t="s" s="2">
         <v>257</v>
       </c>
-      <c r="C8" t="s" s="17">
+      <c r="C8" t="s" s="2">
         <v>258</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" t="s" s="17">
+      <c r="A9" t="s" s="2">
         <v>259</v>
       </c>
-      <c r="B9" t="s" s="17">
+      <c r="B9" t="s" s="2">
         <v>260</v>
       </c>
-      <c r="C9" t="s" s="17">
+      <c r="C9" t="s" s="2">
         <v>261</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" t="s" s="17">
+      <c r="A10" t="s" s="2">
         <v>262</v>
       </c>
-      <c r="B10" t="s" s="17">
+      <c r="B10" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="C10" t="s" s="17">
+      <c r="C10" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" t="s" s="17">
+      <c r="A11" t="s" s="2">
         <v>265</v>
       </c>
-      <c r="B11" t="s" s="17">
+      <c r="B11" t="s" s="2">
         <v>266</v>
       </c>
-      <c r="C11" t="s" s="17">
+      <c r="C11" t="s" s="2">
         <v>266</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" ht="13.65" customHeight="1">
-      <c r="A12" t="s" s="17">
+      <c r="A12" t="s" s="2">
         <v>267</v>
       </c>
-      <c r="B12" t="s" s="17">
+      <c r="B12" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="C12" t="s" s="17">
+      <c r="C12" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" ht="13.65" customHeight="1">
-      <c r="A13" t="s" s="17">
+      <c r="A13" t="s" s="2">
         <v>270</v>
       </c>
-      <c r="B13" t="s" s="17">
+      <c r="B13" t="s" s="2">
         <v>271</v>
       </c>
-      <c r="C13" t="s" s="17">
+      <c r="C13" t="s" s="2">
         <v>272</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" ht="13.65" customHeight="1">
-      <c r="A14" t="s" s="17">
+      <c r="A14" t="s" s="2">
         <v>273</v>
       </c>
-      <c r="B14" t="s" s="17">
+      <c r="B14" t="s" s="2">
         <v>274</v>
       </c>
-      <c r="C14" t="s" s="17">
+      <c r="C14" t="s" s="2">
         <v>275</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" ht="13.65" customHeight="1">
-      <c r="A15" t="s" s="17">
+      <c r="A15" t="s" s="2">
         <v>276</v>
       </c>
-      <c r="B15" t="s" s="17">
+      <c r="B15" t="s" s="2">
         <v>277</v>
       </c>
-      <c r="C15" t="s" s="17">
+      <c r="C15" t="s" s="2">
         <v>278</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" ht="13.65" customHeight="1">
-      <c r="A16" t="s" s="17">
+      <c r="A16" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="B16" t="s" s="17">
+      <c r="B16" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="C16" t="s" s="17">
+      <c r="C16" t="s" s="2">
         <v>281</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" ht="13.65" customHeight="1">
-      <c r="A17" t="s" s="17">
+      <c r="A17" t="s" s="2">
         <v>282</v>
       </c>
-      <c r="B17" t="s" s="17">
+      <c r="B17" t="s" s="2">
         <v>283</v>
       </c>
-      <c r="C17" t="s" s="17">
+      <c r="C17" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" ht="13.65" customHeight="1">
-      <c r="A18" t="s" s="17">
+      <c r="A18" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="B18" t="s" s="17">
+      <c r="B18" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="C18" t="s" s="17">
+      <c r="C18" t="s" s="2">
         <v>287</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" ht="13.65" customHeight="1">
-      <c r="A19" t="s" s="17">
+      <c r="A19" t="s" s="2">
         <v>288</v>
       </c>
-      <c r="B19" t="s" s="17">
+      <c r="B19" t="s" s="2">
         <v>289</v>
       </c>
-      <c r="C19" t="s" s="17">
+      <c r="C19" t="s" s="2">
         <v>290</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17509,9 +17503,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="37.1719" style="19" customWidth="1"/>
-    <col min="2" max="5" width="14.5" style="19" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="19" customWidth="1"/>
+    <col min="1" max="1" width="37.1719" style="17" customWidth="1"/>
+    <col min="2" max="5" width="14.5" style="17" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -17696,9 +17690,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="35" style="20" customWidth="1"/>
-    <col min="2" max="5" width="14.5" style="20" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="20" customWidth="1"/>
+    <col min="1" max="1" width="35" style="18" customWidth="1"/>
+    <col min="2" max="5" width="14.5" style="18" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -17731,7 +17725,7 @@
       <c r="D2" t="s" s="2">
         <v>213</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="19">
         <v>1</v>
       </c>
     </row>
@@ -17763,7 +17757,7 @@
       <c r="D4" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="19">
         <v>1</v>
       </c>
     </row>
@@ -17795,7 +17789,7 @@
       <c r="D6" t="s" s="2">
         <v>223</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
         <v>1</v>
       </c>
     </row>
@@ -17812,7 +17806,7 @@
       <c r="D7" t="s" s="2">
         <v>225</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="19">
         <v>1</v>
       </c>
     </row>
@@ -17844,7 +17838,7 @@
       <c r="D9" t="s" s="2">
         <v>231</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="19">
         <v>1</v>
       </c>
     </row>
@@ -17876,7 +17870,7 @@
       <c r="D11" t="s" s="2">
         <v>237</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="19">
         <v>1</v>
       </c>
     </row>

</xml_diff>